<commit_message>
Modified part1 so it became more space efficent
</commit_message>
<xml_diff>
--- a/Data/Tabelas.xlsx
+++ b/Data/Tabelas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arquivos de Pedro Henrique\Área de Trabalho\Estudos_diversos\Portfólio\Data_Science\Projeto4_BRFSS_Social_Survey\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arquivos de Pedro Henrique\Área de Trabalho\Estudos_diversos\Portfólio\Data_Science\Projeto4_BRFSS_Social_Survey\BRFSS-Social-Survey-2021-Analysis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37FCCEB-B62F-42D2-A2A2-BA8F368D8E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABBE781-1166-4DC9-A48B-12C80C2EBD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="8" xr2:uid="{7DE3C724-4E5C-4829-B9DF-B123A9EE2F37}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{7DE3C724-4E5C-4829-B9DF-B123A9EE2F37}"/>
   </bookViews>
   <sheets>
     <sheet name="Asthma Status" sheetId="2" r:id="rId1"/>
@@ -889,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ACE7292-DDE3-410C-82FC-07AB224B7775}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,6 +984,12 @@
         <v>113</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>3  + 1</f>
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -991,10 +997,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F761288E-F3B0-4E44-A600-6EFA202C9895}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1168,6 +1174,12 @@
         <v>113</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f xml:space="preserve"> 8 +'Asthma Status'!A8</f>
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1176,10 +1188,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F26C3D4B-7778-495C-8FEB-838507BD77E8}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,6 +1266,12 @@
         <v>113</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f xml:space="preserve"> 2 +Demographics!A13</f>
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1261,10 +1279,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F730FCF-54A7-4CB8-8643-603026EFDBF8}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,6 +1428,12 @@
         <v>113</v>
       </c>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f xml:space="preserve"> 6 +Exercise!A7</f>
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1418,10 +1442,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F58B1B6-431C-4645-AD00-9E7E184BB81B}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:B15"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,6 +1690,12 @@
         <v>113</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f xml:space="preserve"> 12 +'Health Status'!A11</f>
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1673,10 +1703,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9DD75C-BA5E-4143-859F-82E39CC7B033}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1842,6 +1872,12 @@
         <v>113</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f xml:space="preserve"> 7 +'Tobbaco USe'!A17</f>
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1852,7 +1888,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="A6:B6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1948,7 +1984,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+      <c r="A8" s="3">
+        <f xml:space="preserve"> 3 +'Alcohol Consumption'!A12</f>
+        <v>42</v>
+      </c>
       <c r="B8"/>
     </row>
   </sheetData>
@@ -1958,10 +1997,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7F2F2E-729E-4B73-9533-6A33342E8517}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2070,6 +2109,12 @@
         <v>113</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f xml:space="preserve"> 4 +'Drugs and Marijuana Use'!A8</f>
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2077,10 +2122,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34F2BC6-0D2D-44CE-BFE4-ED48809FF0D6}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" activeCellId="1" sqref="A5:B5 C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2159,6 +2204,12 @@
         <v>113</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f xml:space="preserve"> 2 +Immunization!A9</f>
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Started exploratory data Analysis
</commit_message>
<xml_diff>
--- a/Data/Tabelas.xlsx
+++ b/Data/Tabelas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arquivos de Pedro Henrique\Área de Trabalho\Estudos_diversos\Portfólio\Data_Science\Projeto4_BRFSS_Social_Survey\BRFSS-Social-Survey-2021-Analysis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABBE781-1166-4DC9-A48B-12C80C2EBD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8B5AB3-9AE7-478E-8901-7CDEF43278D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{7DE3C724-4E5C-4829-B9DF-B123A9EE2F37}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{7DE3C724-4E5C-4829-B9DF-B123A9EE2F37}"/>
   </bookViews>
   <sheets>
     <sheet name="Asthma Status" sheetId="2" r:id="rId1"/>
@@ -468,10 +468,10 @@
     <t>PNEUMO3</t>
   </si>
   <si>
-    <t>METSTAT</t>
-  </si>
-  <si>
     <t>URBSTAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -892,7 +892,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,10 +997,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F761288E-F3B0-4E44-A600-6EFA202C9895}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1180,6 +1180,20 @@
         <v>12</v>
       </c>
     </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f>_xlfn.TEXTJOIN(",
+",TRUE,A2:A9)</f>
+        <v>SEXVAR,
+INCOME3,
+AGEG5YR,
+WTKG3,
+HTM4,
+BMI5 ,
+BMI5CAT,
+RFBMI5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1188,10 +1202,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F26C3D4B-7778-495C-8FEB-838507BD77E8}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,6 +1286,14 @@
         <v>14</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>_xlfn.TEXTJOIN(",
+",TRUE,A2:A3)</f>
+        <v>EXERANY2,
+TOTINDA</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1279,430 +1301,6 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F730FCF-54A7-4CB8-8643-603026EFDBF8}">
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" style="12" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="35" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f xml:space="preserve"> 6 +Exercise!A7</f>
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F58B1B6-431C-4645-AD00-9E7E184BB81B}">
-  <dimension ref="A1:F17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="57.85546875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="35" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" t="s">
-        <v>96</v>
-      </c>
-      <c r="E9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" t="s">
-        <v>96</v>
-      </c>
-      <c r="E10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" t="s">
-        <v>97</v>
-      </c>
-      <c r="E12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" t="s">
-        <v>91</v>
-      </c>
-      <c r="E13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B15" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f xml:space="preserve"> 12 +'Health Status'!A11</f>
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9DD75C-BA5E-4143-859F-82E39CC7B033}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1739,58 +1337,227 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>48</v>
+        <v>20</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E2" t="s">
         <v>77</v>
       </c>
-      <c r="F2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>50</v>
+        <v>22</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>88</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E3" t="s">
         <v>77</v>
       </c>
       <c r="F3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>52</v>
+        <v>24</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="C4" t="s">
         <v>88</v>
       </c>
       <c r="D4" t="s">
-        <v>100</v>
+        <v>91</v>
+      </c>
+      <c r="E4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f xml:space="preserve"> 6 +Exercise!A7</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f>_xlfn.TEXTJOIN(",
+",TRUE,A2:A7)</f>
+        <v>GENHLTH,
+PHYSHLTH,
+DIFFWALK,
+DIFFALON,
+RFHLTH,
+PHYS14D</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F58B1B6-431C-4645-AD00-9E7E184BB81B}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="57.85546875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="35" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
+        <v>91</v>
       </c>
       <c r="E4" t="s">
         <v>77</v>
@@ -1798,16 +1565,16 @@
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>120</v>
+        <v>35</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="E5" t="s">
         <v>77</v>
@@ -1815,13 +1582,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>55</v>
+        <v>117</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
         <v>95</v>
@@ -1830,29 +1597,29 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
         <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
         <v>75</v>
@@ -1864,18 +1631,121 @@
         <v>77</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" t="s">
+        <v>77</v>
+      </c>
+    </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B15" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f xml:space="preserve"> 7 +'Tobbaco USe'!A17</f>
-        <v>39</v>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f xml:space="preserve"> 12 +'Health Status'!A11</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f>_xlfn.TEXTJOIN(",
+",TRUE,A2:A13)</f>
+        <v xml:space="preserve"> SMOKE100,
+ SMOKDAY2,
+USENOW3,
+ECIGNOW1,
+SMOKER3,
+RFSMOK3,
+CURECI1,
+LCSFIRST,
+ LCSLAST,
+ LCSNUMCG,
+LASTSMK2,
+ STOPSMK2</v>
       </c>
     </row>
   </sheetData>
@@ -1883,12 +1753,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C7C4E0-2F59-4726-A02D-EF606F7B0B59}">
-  <dimension ref="A1:F8"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9DD75C-BA5E-4143-859F-82E39CC7B033}">
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,30 +1793,33 @@
     </row>
     <row r="2" spans="1:6" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
         <v>97</v>
@@ -1958,45 +1831,125 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>62</v>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="E4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B10" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <f xml:space="preserve"> 3 +'Alcohol Consumption'!A12</f>
-        <v>42</v>
-      </c>
-      <c r="B8"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f xml:space="preserve"> 7 +'Tobbaco USe'!A17</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f>_xlfn.TEXTJOIN(",
+",TRUE,A2:A8)</f>
+        <v>ALCDAY5,
+AVEDRNK3,
+DRNKANY5,
+DROCDY3,
+RFBING5,
+DRNKWK1,
+RFDRHV7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7F2F2E-729E-4B73-9533-6A33342E8517}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C7C4E0-2F59-4726-A02D-EF606F7B0B59}">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2033,6 +1986,127 @@
         <v>92</v>
       </c>
     </row>
+    <row r="2" spans="1:6" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <f xml:space="preserve"> 3 +'Alcohol Consumption'!A12</f>
+        <v>42</v>
+      </c>
+      <c r="B8"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>_xlfn.TEXTJOIN(",
+",TRUE,A2:A4)</f>
+        <v>ACEDRUGS,
+MARIJAN1,
+RSNMRJN2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7F2F2E-729E-4B73-9533-6A33342E8517}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="35" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>65</v>
@@ -2113,6 +2187,16 @@
       <c r="A9">
         <f xml:space="preserve"> 4 +'Drugs and Marijuana Use'!A8</f>
         <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>_xlfn.TEXTJOIN(",
+",TRUE,A2:A5)</f>
+        <v>FLUSHOT7,
+PNEUVAC4,
+FLSHOT7,
+PNEUMO3</v>
       </c>
     </row>
   </sheetData>
@@ -2122,10 +2206,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34F2BC6-0D2D-44CE-BFE4-ED48809FF0D6}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2160,7 +2244,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>70</v>
@@ -2177,7 +2261,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>71</v>
@@ -2210,6 +2294,14 @@
         <v>48</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>_xlfn.TEXTJOIN(",
+",TRUE,A2:A3)</f>
+        <v xml:space="preserve"> ,
+URBSTAT</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modified Urban rural, made average days for Physical Health
</commit_message>
<xml_diff>
--- a/Data/Tabelas.xlsx
+++ b/Data/Tabelas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arquivos de Pedro Henrique\Área de Trabalho\Estudos_diversos\Portfólio\Data_Science\Projeto4_BRFSS_Social_Survey\BRFSS-Social-Survey-2021-Analysis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D9E758-48F0-4EBC-A9DA-8168408E7051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883FB39E-AC02-4B69-819F-C301E96E9F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{7DE3C724-4E5C-4829-B9DF-B123A9EE2F37}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{7DE3C724-4E5C-4829-B9DF-B123A9EE2F37}"/>
   </bookViews>
   <sheets>
     <sheet name="Asthma Status" sheetId="2" r:id="rId1"/>
@@ -1000,7 +1000,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1304,7 +1304,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,7 +1478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F58B1B6-431C-4645-AD00-9E7E184BB81B}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -2073,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7F2F2E-729E-4B73-9533-6A33342E8517}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2209,7 +2209,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finished Health Status and Tobbaco use
</commit_message>
<xml_diff>
--- a/Data/Tabelas.xlsx
+++ b/Data/Tabelas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arquivos de Pedro Henrique\Área de Trabalho\Estudos_diversos\Portfólio\Data_Science\Projeto4_BRFSS_Social_Survey\BRFSS-Social-Survey-2021-Analysis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883FB39E-AC02-4B69-819F-C301E96E9F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FD55DE-4F4D-4B4D-A413-862F6649C742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{7DE3C724-4E5C-4829-B9DF-B123A9EE2F37}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{7DE3C724-4E5C-4829-B9DF-B123A9EE2F37}"/>
   </bookViews>
   <sheets>
     <sheet name="Asthma Status" sheetId="2" r:id="rId1"/>
@@ -1000,7 +1000,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1204,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F26C3D4B-7778-495C-8FEB-838507BD77E8}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1304,7 +1304,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1479,7 +1479,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2073,7 +2073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7F2F2E-729E-4B73-9533-6A33342E8517}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>